<commit_message>
vytvorenie formularov - vsetky kroky
</commit_message>
<xml_diff>
--- a/formulare-udaje.xlsx
+++ b/formulare-udaje.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barborka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barborka\Desktop\skola\ICP\prototyp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>